<commit_message>
color coded new elections with shapefile status
</commit_message>
<xml_diff>
--- a/acs/elections.xlsx
+++ b/acs/elections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Downloads\RA Work\acs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kguan17/Documents/GitHub/RA-Work/acs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1890992E-C75C-4BCC-A695-A562187F1CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A05CAEF-C5B8-5D4B-959A-AFAAF6E24DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="4215" windowWidth="21555" windowHeight="11385" xr2:uid="{6B2EB732-C0BF-4336-8C6B-FF3332FBF24E}"/>
+    <workbookView xWindow="-6920" yWindow="-28300" windowWidth="21560" windowHeight="28300" xr2:uid="{6B2EB732-C0BF-4336-8C6B-FF3332FBF24E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="545">
   <si>
     <t>filename</t>
   </si>
@@ -1668,6 +1668,9 @@
   </si>
   <si>
     <t>takoma_park_wards_2022.csv</t>
+  </si>
+  <si>
+    <t>corvallis_city_council_2022.csv</t>
   </si>
 </sst>
 </file>
@@ -2048,21 +2051,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022FCB54-8620-44BA-9E5B-DD50E1770DCA}">
   <dimension ref="A1:H410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
-      <selection activeCell="D357" sqref="D357"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="68.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
     <col min="3" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2088,7 +2091,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>203</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>205</v>
       </c>
@@ -2134,7 +2137,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>206</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>207</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>208</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>260</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>261</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>68</v>
       </c>
@@ -2270,7 +2273,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>77</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>90</v>
       </c>
@@ -2333,7 +2336,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>91</v>
       </c>
@@ -2354,7 +2357,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>102</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>103</v>
       </c>
@@ -2396,7 +2399,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>104</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>109</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>110</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>111</v>
       </c>
@@ -2480,7 +2483,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>112</v>
       </c>
@@ -2501,7 +2504,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>119</v>
       </c>
@@ -2522,7 +2525,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>147</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>148</v>
       </c>
@@ -2564,7 +2567,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>155</v>
       </c>
@@ -2585,7 +2588,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>161</v>
       </c>
@@ -2606,7 +2609,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>180</v>
       </c>
@@ -2627,7 +2630,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>199</v>
       </c>
@@ -2648,7 +2651,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>200</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>201</v>
       </c>
@@ -2690,7 +2693,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>209</v>
       </c>
@@ -2711,7 +2714,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>257</v>
       </c>
@@ -2732,7 +2735,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>258</v>
       </c>
@@ -2755,7 +2758,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>268</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>269</v>
       </c>
@@ -2797,7 +2800,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>273</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>276</v>
       </c>
@@ -2839,7 +2842,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>278</v>
       </c>
@@ -2860,7 +2863,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>287</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>291</v>
       </c>
@@ -2902,7 +2905,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>295</v>
       </c>
@@ -2923,7 +2926,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>296</v>
       </c>
@@ -2944,7 +2947,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>305</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>309</v>
       </c>
@@ -2986,7 +2989,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>316</v>
       </c>
@@ -3007,7 +3010,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>323</v>
       </c>
@@ -3028,7 +3031,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>327</v>
       </c>
@@ -3049,7 +3052,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>336</v>
       </c>
@@ -3070,7 +3073,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>338</v>
       </c>
@@ -3091,7 +3094,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>339</v>
       </c>
@@ -3112,7 +3115,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>373</v>
       </c>
@@ -3133,7 +3136,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>374</v>
       </c>
@@ -3154,7 +3157,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>376</v>
       </c>
@@ -3175,7 +3178,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>379</v>
       </c>
@@ -3196,7 +3199,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>391</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>392</v>
       </c>
@@ -3238,7 +3241,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>393</v>
       </c>
@@ -3259,7 +3262,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>394</v>
       </c>
@@ -3280,7 +3283,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>395</v>
       </c>
@@ -3301,7 +3304,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>406</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>407</v>
       </c>
@@ -3343,7 +3346,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>411</v>
       </c>
@@ -3364,7 +3367,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>417</v>
       </c>
@@ -3385,7 +3388,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>424</v>
       </c>
@@ -3406,7 +3409,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>428</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>430</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>437</v>
       </c>
@@ -3469,7 +3472,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>438</v>
       </c>
@@ -3490,7 +3493,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>439</v>
       </c>
@@ -3511,7 +3514,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>440</v>
       </c>
@@ -3532,7 +3535,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
@@ -3558,7 +3561,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
@@ -3584,7 +3587,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
@@ -3610,7 +3613,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>75</v>
       </c>
@@ -3636,7 +3639,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>76</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>79</v>
       </c>
@@ -3688,7 +3691,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>80</v>
       </c>
@@ -3714,7 +3717,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>81</v>
       </c>
@@ -3740,7 +3743,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
@@ -3792,7 +3795,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>84</v>
       </c>
@@ -3818,7 +3821,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -3844,7 +3847,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>86</v>
       </c>
@@ -3870,7 +3873,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>87</v>
       </c>
@@ -3896,7 +3899,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
@@ -3922,7 +3925,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>89</v>
       </c>
@@ -3948,7 +3951,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>94</v>
       </c>
@@ -3974,7 +3977,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>95</v>
       </c>
@@ -4000,7 +4003,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>96</v>
       </c>
@@ -4026,7 +4029,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>97</v>
       </c>
@@ -4052,7 +4055,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>98</v>
       </c>
@@ -4078,7 +4081,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>99</v>
       </c>
@@ -4104,7 +4107,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>100</v>
       </c>
@@ -4130,7 +4133,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>101</v>
       </c>
@@ -4156,7 +4159,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>105</v>
       </c>
@@ -4182,7 +4185,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>106</v>
       </c>
@@ -4208,7 +4211,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>107</v>
       </c>
@@ -4234,30 +4237,33 @@
         <v>533</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="E97" s="3">
+      <c r="D97" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="E97" s="1">
         <v>9</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G97" s="3">
+      <c r="F97" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G97" s="1">
         <v>2022</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>117</v>
       </c>
@@ -4283,7 +4289,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>118</v>
       </c>
@@ -4309,7 +4315,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>133</v>
       </c>
@@ -4335,7 +4341,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>134</v>
       </c>
@@ -4361,7 +4367,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>135</v>
       </c>
@@ -4387,7 +4393,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>136</v>
       </c>
@@ -4413,7 +4419,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>137</v>
       </c>
@@ -4439,7 +4445,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>138</v>
       </c>
@@ -4465,7 +4471,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>139</v>
       </c>
@@ -4491,7 +4497,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>140</v>
       </c>
@@ -4517,7 +4523,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>141</v>
       </c>
@@ -4543,7 +4549,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>142</v>
       </c>
@@ -4569,7 +4575,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>143</v>
       </c>
@@ -4595,7 +4601,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>144</v>
       </c>
@@ -4621,7 +4627,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>145</v>
       </c>
@@ -4647,7 +4653,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>146</v>
       </c>
@@ -4673,7 +4679,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>158</v>
       </c>
@@ -4699,7 +4705,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>159</v>
       </c>
@@ -4725,7 +4731,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>160</v>
       </c>
@@ -4751,7 +4757,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>167</v>
       </c>
@@ -4777,7 +4783,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>168</v>
       </c>
@@ -4803,7 +4809,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>169</v>
       </c>
@@ -4829,7 +4835,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>170</v>
       </c>
@@ -4855,7 +4861,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>171</v>
       </c>
@@ -4881,7 +4887,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>172</v>
       </c>
@@ -4907,7 +4913,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>173</v>
       </c>
@@ -4933,7 +4939,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>174</v>
       </c>
@@ -4959,7 +4965,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>175</v>
       </c>
@@ -4985,7 +4991,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>176</v>
       </c>
@@ -5011,7 +5017,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>177</v>
       </c>
@@ -5037,7 +5043,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>178</v>
       </c>
@@ -5063,7 +5069,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>179</v>
       </c>
@@ -5089,7 +5095,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>187</v>
       </c>
@@ -5115,7 +5121,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>188</v>
       </c>
@@ -5141,7 +5147,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>189</v>
       </c>
@@ -5167,7 +5173,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>190</v>
       </c>
@@ -5193,7 +5199,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>191</v>
       </c>
@@ -5219,7 +5225,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>192</v>
       </c>
@@ -5245,7 +5251,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>193</v>
       </c>
@@ -5271,7 +5277,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>194</v>
       </c>
@@ -5297,7 +5303,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>195</v>
       </c>
@@ -5323,7 +5329,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>196</v>
       </c>
@@ -5349,7 +5355,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>197</v>
       </c>
@@ -5375,7 +5381,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>198</v>
       </c>
@@ -5401,7 +5407,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>202</v>
       </c>
@@ -5427,7 +5433,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>211</v>
       </c>
@@ -5453,7 +5459,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>212</v>
       </c>
@@ -5479,7 +5485,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>213</v>
       </c>
@@ -5505,7 +5511,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>214</v>
       </c>
@@ -5531,7 +5537,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>215</v>
       </c>
@@ -5557,7 +5563,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>216</v>
       </c>
@@ -5583,7 +5589,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>217</v>
       </c>
@@ -5609,7 +5615,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>218</v>
       </c>
@@ -5635,7 +5641,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>219</v>
       </c>
@@ -5661,7 +5667,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>220</v>
       </c>
@@ -5687,7 +5693,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>221</v>
       </c>
@@ -5713,7 +5719,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>222</v>
       </c>
@@ -5739,7 +5745,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>223</v>
       </c>
@@ -5765,7 +5771,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>224</v>
       </c>
@@ -5791,7 +5797,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>225</v>
       </c>
@@ -5817,7 +5823,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>226</v>
       </c>
@@ -5843,7 +5849,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>227</v>
       </c>
@@ -5869,7 +5875,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>228</v>
       </c>
@@ -5895,7 +5901,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>229</v>
       </c>
@@ -5921,7 +5927,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>230</v>
       </c>
@@ -5947,7 +5953,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>231</v>
       </c>
@@ -5973,7 +5979,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>232</v>
       </c>
@@ -5999,7 +6005,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>233</v>
       </c>
@@ -6025,7 +6031,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>234</v>
       </c>
@@ -6051,7 +6057,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>235</v>
       </c>
@@ -6077,7 +6083,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>236</v>
       </c>
@@ -6103,7 +6109,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>237</v>
       </c>
@@ -6129,7 +6135,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>238</v>
       </c>
@@ -6155,7 +6161,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>239</v>
       </c>
@@ -6181,7 +6187,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>240</v>
       </c>
@@ -6207,7 +6213,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>241</v>
       </c>
@@ -6233,7 +6239,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>242</v>
       </c>
@@ -6259,7 +6265,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>243</v>
       </c>
@@ -6285,7 +6291,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>244</v>
       </c>
@@ -6311,7 +6317,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>245</v>
       </c>
@@ -6337,7 +6343,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>246</v>
       </c>
@@ -6363,7 +6369,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>247</v>
       </c>
@@ -6389,7 +6395,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>248</v>
       </c>
@@ -6415,7 +6421,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>249</v>
       </c>
@@ -6441,7 +6447,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>250</v>
       </c>
@@ -6467,7 +6473,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>251</v>
       </c>
@@ -6493,7 +6499,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>252</v>
       </c>
@@ -6519,7 +6525,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>253</v>
       </c>
@@ -6545,7 +6551,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>254</v>
       </c>
@@ -6571,7 +6577,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>255</v>
       </c>
@@ -6597,7 +6603,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>256</v>
       </c>
@@ -6623,7 +6629,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>262</v>
       </c>
@@ -6649,7 +6655,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>263</v>
       </c>
@@ -6675,7 +6681,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>264</v>
       </c>
@@ -6701,7 +6707,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>265</v>
       </c>
@@ -6727,7 +6733,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>266</v>
       </c>
@@ -6753,7 +6759,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>267</v>
       </c>
@@ -6779,7 +6785,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>270</v>
       </c>
@@ -6805,7 +6811,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>271</v>
       </c>
@@ -6831,7 +6837,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>272</v>
       </c>
@@ -6857,7 +6863,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>279</v>
       </c>
@@ -6883,7 +6889,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>280</v>
       </c>
@@ -6909,7 +6915,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>281</v>
       </c>
@@ -6935,7 +6941,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>282</v>
       </c>
@@ -6961,7 +6967,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>288</v>
       </c>
@@ -6987,7 +6993,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>289</v>
       </c>
@@ -7013,7 +7019,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>290</v>
       </c>
@@ -7039,7 +7045,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>297</v>
       </c>
@@ -7065,7 +7071,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>298</v>
       </c>
@@ -7091,7 +7097,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>299</v>
       </c>
@@ -7117,7 +7123,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>300</v>
       </c>
@@ -7143,7 +7149,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>306</v>
       </c>
@@ -7169,7 +7175,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>307</v>
       </c>
@@ -7195,7 +7201,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>308</v>
       </c>
@@ -7221,7 +7227,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>312</v>
       </c>
@@ -7247,7 +7253,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>313</v>
       </c>
@@ -7273,7 +7279,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>314</v>
       </c>
@@ -7299,7 +7305,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>315</v>
       </c>
@@ -7325,7 +7331,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>321</v>
       </c>
@@ -7351,7 +7357,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>322</v>
       </c>
@@ -7377,7 +7383,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>342</v>
       </c>
@@ -7403,7 +7409,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>344</v>
       </c>
@@ -7429,7 +7435,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>345</v>
       </c>
@@ -7455,7 +7461,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>346</v>
       </c>
@@ -7481,7 +7487,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>347</v>
       </c>
@@ -7507,7 +7513,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>348</v>
       </c>
@@ -7533,7 +7539,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>349</v>
       </c>
@@ -7559,7 +7565,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>350</v>
       </c>
@@ -7585,7 +7591,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>351</v>
       </c>
@@ -7611,7 +7617,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>352</v>
       </c>
@@ -7637,7 +7643,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>353</v>
       </c>
@@ -7663,7 +7669,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>354</v>
       </c>
@@ -7689,7 +7695,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>358</v>
       </c>
@@ -7715,7 +7721,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>359</v>
       </c>
@@ -7741,7 +7747,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>360</v>
       </c>
@@ -7767,7 +7773,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>361</v>
       </c>
@@ -7793,7 +7799,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>362</v>
       </c>
@@ -7819,7 +7825,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>363</v>
       </c>
@@ -7845,7 +7851,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>364</v>
       </c>
@@ -7871,7 +7877,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>365</v>
       </c>
@@ -7897,7 +7903,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>366</v>
       </c>
@@ -7923,7 +7929,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>367</v>
       </c>
@@ -7949,7 +7955,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>368</v>
       </c>
@@ -7975,7 +7981,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>369</v>
       </c>
@@ -8001,7 +8007,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>370</v>
       </c>
@@ -8027,7 +8033,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>371</v>
       </c>
@@ -8053,7 +8059,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>372</v>
       </c>
@@ -8079,7 +8085,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>375</v>
       </c>
@@ -8105,7 +8111,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>377</v>
       </c>
@@ -8131,7 +8137,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>378</v>
       </c>
@@ -8157,7 +8163,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>381</v>
       </c>
@@ -8183,7 +8189,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>382</v>
       </c>
@@ -8209,7 +8215,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>383</v>
       </c>
@@ -8235,7 +8241,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>384</v>
       </c>
@@ -8261,7 +8267,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>385</v>
       </c>
@@ -8287,7 +8293,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>386</v>
       </c>
@@ -8313,7 +8319,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>387</v>
       </c>
@@ -8339,7 +8345,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>388</v>
       </c>
@@ -8365,7 +8371,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>389</v>
       </c>
@@ -8391,7 +8397,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>390</v>
       </c>
@@ -8417,7 +8423,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>396</v>
       </c>
@@ -8443,7 +8449,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>397</v>
       </c>
@@ -8469,7 +8475,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>398</v>
       </c>
@@ -8495,7 +8501,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>399</v>
       </c>
@@ -8521,7 +8527,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>400</v>
       </c>
@@ -8547,7 +8553,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>401</v>
       </c>
@@ -8573,7 +8579,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>402</v>
       </c>
@@ -8599,7 +8605,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>403</v>
       </c>
@@ -8625,7 +8631,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>404</v>
       </c>
@@ -8651,7 +8657,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>405</v>
       </c>
@@ -8677,7 +8683,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>412</v>
       </c>
@@ -8703,7 +8709,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>413</v>
       </c>
@@ -8729,7 +8735,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>426</v>
       </c>
@@ -8752,7 +8758,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>427</v>
       </c>
@@ -8775,7 +8781,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" s="2" t="s">
         <v>429</v>
       </c>
@@ -8798,7 +8804,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>431</v>
       </c>
@@ -8821,7 +8827,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>432</v>
       </c>
@@ -8844,7 +8850,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>433</v>
       </c>
@@ -8870,7 +8876,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>434</v>
       </c>
@@ -8896,7 +8902,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>435</v>
       </c>
@@ -8922,7 +8928,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>436</v>
       </c>
@@ -8948,7 +8954,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>120</v>
       </c>
@@ -8972,7 +8978,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>130</v>
       </c>
@@ -8996,7 +9002,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>131</v>
       </c>
@@ -9020,7 +9026,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>132</v>
       </c>
@@ -9044,7 +9050,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
         <v>328</v>
       </c>
@@ -9065,7 +9071,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A284" s="2" t="s">
         <v>330</v>
       </c>
@@ -9086,7 +9092,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
         <v>334</v>
       </c>
@@ -9107,7 +9113,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>332</v>
       </c>
@@ -9133,7 +9139,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>409</v>
       </c>
@@ -9159,7 +9165,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>410</v>
       </c>
@@ -9185,7 +9191,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>414</v>
       </c>
@@ -9211,7 +9217,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>415</v>
       </c>
@@ -9237,7 +9243,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
         <v>416</v>
       </c>
@@ -9263,7 +9269,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>418</v>
       </c>
@@ -9289,7 +9295,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
         <v>419</v>
       </c>
@@ -9315,7 +9321,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>420</v>
       </c>
@@ -9341,7 +9347,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
         <v>421</v>
       </c>
@@ -9367,7 +9373,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>422</v>
       </c>
@@ -9393,7 +9399,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
         <v>423</v>
       </c>
@@ -9419,7 +9425,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>425</v>
       </c>
@@ -9445,7 +9451,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
         <v>10</v>
       </c>
@@ -9469,7 +9475,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>12</v>
       </c>
@@ -9493,7 +9499,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
         <v>13</v>
       </c>
@@ -9517,7 +9523,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>14</v>
       </c>
@@ -9541,7 +9547,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
         <v>15</v>
       </c>
@@ -9565,7 +9571,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>16</v>
       </c>
@@ -9589,7 +9595,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
         <v>17</v>
       </c>
@@ -9613,7 +9619,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>18</v>
       </c>
@@ -9637,7 +9643,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
         <v>19</v>
       </c>
@@ -9661,7 +9667,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>20</v>
       </c>
@@ -9685,7 +9691,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
         <v>21</v>
       </c>
@@ -9709,7 +9715,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>22</v>
       </c>
@@ -9733,7 +9739,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
         <v>23</v>
       </c>
@@ -9757,7 +9763,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>24</v>
       </c>
@@ -9781,7 +9787,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
         <v>25</v>
       </c>
@@ -9805,7 +9811,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
         <v>26</v>
       </c>
@@ -9829,7 +9835,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A315" s="1" t="s">
         <v>27</v>
       </c>
@@ -9853,7 +9859,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
         <v>28</v>
       </c>
@@ -9877,7 +9883,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
         <v>29</v>
       </c>
@@ -9901,7 +9907,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
         <v>30</v>
       </c>
@@ -9925,7 +9931,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
         <v>31</v>
       </c>
@@ -9949,7 +9955,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>32</v>
       </c>
@@ -9973,7 +9979,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
         <v>33</v>
       </c>
@@ -9997,7 +10003,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>34</v>
       </c>
@@ -10021,7 +10027,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
         <v>35</v>
       </c>
@@ -10045,7 +10051,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>36</v>
       </c>
@@ -10069,7 +10075,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>37</v>
       </c>
@@ -10093,7 +10099,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>38</v>
       </c>
@@ -10117,7 +10123,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
         <v>39</v>
       </c>
@@ -10141,7 +10147,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
         <v>40</v>
       </c>
@@ -10165,7 +10171,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
         <v>41</v>
       </c>
@@ -10189,7 +10195,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>42</v>
       </c>
@@ -10213,7 +10219,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
         <v>43</v>
       </c>
@@ -10237,7 +10243,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
         <v>44</v>
       </c>
@@ -10261,7 +10267,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
         <v>123</v>
       </c>
@@ -10285,7 +10291,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>125</v>
       </c>
@@ -10309,7 +10315,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
         <v>126</v>
       </c>
@@ -10333,7 +10339,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
         <v>127</v>
       </c>
@@ -10357,7 +10363,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A337" s="2" t="s">
         <v>343</v>
       </c>
@@ -10378,7 +10384,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A338" s="2" t="s">
         <v>355</v>
       </c>
@@ -10399,7 +10405,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
         <v>150</v>
       </c>
@@ -10425,7 +10431,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>151</v>
       </c>
@@ -10451,7 +10457,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A341" s="1" t="s">
         <v>152</v>
       </c>
@@ -10477,7 +10483,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
         <v>153</v>
       </c>
@@ -10503,7 +10509,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
         <v>154</v>
       </c>
@@ -10529,7 +10535,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
         <v>156</v>
       </c>
@@ -10555,7 +10561,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A345" s="1" t="s">
         <v>157</v>
       </c>
@@ -10581,7 +10587,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
         <v>162</v>
       </c>
@@ -10607,7 +10613,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
         <v>163</v>
       </c>
@@ -10633,7 +10639,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
         <v>164</v>
       </c>
@@ -10659,7 +10665,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
         <v>165</v>
       </c>
@@ -10685,7 +10691,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>166</v>
       </c>
@@ -10711,7 +10717,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
         <v>181</v>
       </c>
@@ -10737,7 +10743,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>182</v>
       </c>
@@ -10763,7 +10769,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
         <v>183</v>
       </c>
@@ -10789,7 +10795,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>184</v>
       </c>
@@ -10815,7 +10821,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
         <v>185</v>
       </c>
@@ -10841,7 +10847,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>186</v>
       </c>
@@ -10867,7 +10873,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A357" s="2" t="s">
         <v>340</v>
       </c>
@@ -10888,7 +10894,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A358" s="2" t="s">
         <v>341</v>
       </c>
@@ -10909,7 +10915,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>274</v>
       </c>
@@ -10935,7 +10941,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>283</v>
       </c>
@@ -10961,7 +10967,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
         <v>284</v>
       </c>
@@ -10987,7 +10993,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
         <v>285</v>
       </c>
@@ -11013,7 +11019,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="s">
         <v>286</v>
       </c>
@@ -11039,7 +11045,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>292</v>
       </c>
@@ -11065,7 +11071,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
         <v>293</v>
       </c>
@@ -11091,7 +11097,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>294</v>
       </c>
@@ -11117,7 +11123,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
         <v>301</v>
       </c>
@@ -11143,7 +11149,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
         <v>302</v>
       </c>
@@ -11169,7 +11175,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A369" s="1" t="s">
         <v>303</v>
       </c>
@@ -11195,7 +11201,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
         <v>304</v>
       </c>
@@ -11221,7 +11227,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
         <v>310</v>
       </c>
@@ -11247,7 +11253,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A372" s="1" t="s">
         <v>311</v>
       </c>
@@ -11273,7 +11279,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A373" s="1" t="s">
         <v>317</v>
       </c>
@@ -11299,7 +11305,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
         <v>318</v>
       </c>
@@ -11325,7 +11331,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
         <v>319</v>
       </c>
@@ -11351,7 +11357,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
         <v>320</v>
       </c>
@@ -11377,7 +11383,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
         <v>324</v>
       </c>
@@ -11403,7 +11409,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
         <v>325</v>
       </c>
@@ -11429,7 +11435,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
         <v>326</v>
       </c>
@@ -11455,7 +11461,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A380" s="2" t="s">
         <v>356</v>
       </c>
@@ -11476,7 +11482,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A381" s="2" t="s">
         <v>3</v>
       </c>
@@ -11495,7 +11501,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A382" s="2" t="s">
         <v>5</v>
       </c>
@@ -11514,7 +11520,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A383" s="2" t="s">
         <v>8</v>
       </c>
@@ -11533,7 +11539,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A384" s="2" t="s">
         <v>65</v>
       </c>
@@ -11552,7 +11558,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A385" s="2" t="s">
         <v>66</v>
       </c>
@@ -11571,7 +11577,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A386" s="2" t="s">
         <v>113</v>
       </c>
@@ -11590,7 +11596,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A387" s="2" t="s">
         <v>114</v>
       </c>
@@ -11609,7 +11615,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A388" s="2" t="s">
         <v>115</v>
       </c>
@@ -11628,7 +11634,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A389" s="2" t="s">
         <v>116</v>
       </c>
@@ -11647,7 +11653,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A390" s="2" t="s">
         <v>121</v>
       </c>
@@ -11666,7 +11672,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A391" s="2" t="s">
         <v>441</v>
       </c>
@@ -11685,7 +11691,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A392" s="1" t="s">
         <v>45</v>
       </c>
@@ -11709,7 +11715,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A393" s="1" t="s">
         <v>48</v>
       </c>
@@ -11733,7 +11739,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
         <v>49</v>
       </c>
@@ -11757,7 +11763,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
         <v>50</v>
       </c>
@@ -11781,7 +11787,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
         <v>51</v>
       </c>
@@ -11805,7 +11811,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A397" s="1" t="s">
         <v>52</v>
       </c>
@@ -11829,7 +11835,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
         <v>53</v>
       </c>
@@ -11853,7 +11859,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A399" s="1" t="s">
         <v>54</v>
       </c>
@@ -11877,7 +11883,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A400" s="1" t="s">
         <v>55</v>
       </c>
@@ -11901,7 +11907,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A401" s="1" t="s">
         <v>56</v>
       </c>
@@ -11925,7 +11931,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A402" s="1" t="s">
         <v>57</v>
       </c>
@@ -11949,7 +11955,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
         <v>58</v>
       </c>
@@ -11973,7 +11979,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
         <v>59</v>
       </c>
@@ -11997,7 +12003,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A405" s="1" t="s">
         <v>60</v>
       </c>
@@ -12021,7 +12027,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
         <v>61</v>
       </c>
@@ -12045,7 +12051,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A407" s="1" t="s">
         <v>62</v>
       </c>
@@ -12069,7 +12075,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
         <v>63</v>
       </c>
@@ -12093,7 +12099,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
         <v>64</v>
       </c>
@@ -12117,7 +12123,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
         <v>128</v>
       </c>

</xml_diff>